<commit_message>
registration screen is added to Glossary
</commit_message>
<xml_diff>
--- a/DesignDocs/Glossary_Random4Dinner.xlsx
+++ b/DesignDocs/Glossary_Random4Dinner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EnyFood\Random4Dinner\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF391D0B-9E08-4BF2-907E-C9F0D58B2B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7800F3-6B38-428E-8712-7CA98BE0E56E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38025" yWindow="645" windowWidth="34260" windowHeight="20085" xr2:uid="{8C7EFB95-537E-4066-989B-733ADEACC89B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Random4Dinner</t>
   </si>
@@ -156,6 +156,14 @@
     <t>1. Edit button
 2. Stepper
 3. Counter</t>
+  </si>
+  <si>
+    <t>"Registration" screen</t>
+  </si>
+  <si>
+    <t>1. [Войти через Google] button
+2. [Зарегистрироваться] button
+3. [Продолжить без регистрации] button</t>
   </si>
 </sst>
 </file>
@@ -264,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -277,9 +285,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -288,6 +293,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -312,14 +324,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2760345</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>2764155</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1905</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -362,13 +374,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2918094</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:colOff>2914284</xdr:colOff>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>4342857</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -406,13 +418,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2934094</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -456,14 +468,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>19399</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>11972</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1905</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -500,13 +512,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>4283667</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -550,14 +562,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2722245</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>4130040</xdr:rowOff>
+      <xdr:colOff>2726055</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>4131945</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -600,14 +612,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2914650</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>4379751</xdr:rowOff>
+      <xdr:colOff>2910840</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>4381656</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -650,14 +662,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2974213</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>4419601</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>4421506</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -700,14 +712,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>4435637</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>4441352</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -750,14 +762,14 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>201047</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>3105149</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>3108959</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>4627245</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -800,14 +812,14 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>19644</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>4419600</xdr:rowOff>
+      <xdr:colOff>15834</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>4421505</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -850,14 +862,14 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>3105150</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>4625340</xdr:rowOff>
+      <xdr:colOff>3101340</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>4631055</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -892,6 +904,67 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2802960</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>4141470</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Рисунок 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DF3A1BE-732D-461C-BD89-54EDF8D984F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="504825"/>
+          <a:ext cx="2799150" cy="4143375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1196,10 +1269,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3B538B-1E03-4212-A4DA-A3DBB822E499}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1225,111 +1298,124 @@
       </c>
       <c r="B1" s="5"/>
     </row>
-    <row r="2" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:13" s="10" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="9"/>
+    </row>
+    <row r="3" spans="1:13" s="10" customFormat="1" ht="327.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3"/>
+      <c r="B3" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
+      <c r="B4" s="9"/>
     </row>
-    <row r="3" spans="1:13" ht="328.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="3" t="s">
+    <row r="5" spans="1:13" ht="328.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+    <row r="6" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6" t="s">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6" t="s">
+      <c r="D6" s="9"/>
+      <c r="E6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="6"/>
+      <c r="F6" s="9"/>
     </row>
-    <row r="5" spans="1:13" ht="342" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
+    <row r="7" spans="1:13" ht="342" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="6"/>
-    </row>
-    <row r="7" spans="1:13" ht="339" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="9"/>
+    </row>
+    <row r="9" spans="1:13" ht="339" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="7" t="s">
+      <c r="B10" s="7"/>
+      <c r="C10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="7" t="s">
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="7" t="s">
+      <c r="H10" s="7"/>
+      <c r="I10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="8"/>
-      <c r="K8" s="7" t="s">
+      <c r="J10" s="7"/>
+      <c r="K10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="9"/>
-      <c r="M8" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="7"/>
     </row>
-    <row r="9" spans="1:13" ht="365.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
+    <row r="11" spans="1:13" ht="365.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="M11" s="3" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="I8:J8"/>
+  <mergeCells count="11">
     <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A6:B6"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="C10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
E2E test documentation start
</commit_message>
<xml_diff>
--- a/DesignDocs/Glossary_Random4Dinner.xlsx
+++ b/DesignDocs/Glossary_Random4Dinner.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EnyFood\Random4Dinner\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7800F3-6B38-428E-8712-7CA98BE0E56E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5624E8B-E9BF-4F03-8CCA-CADC59E8BBB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38025" yWindow="645" windowWidth="34260" windowHeight="20085" xr2:uid="{8C7EFB95-537E-4066-989B-733ADEACC89B}"/>
+    <workbookView xWindow="-25740" yWindow="1080" windowWidth="24960" windowHeight="20085" xr2:uid="{8C7EFB95-537E-4066-989B-733ADEACC89B}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист2" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Random4Dinner</t>
   </si>
@@ -55,37 +55,7 @@
     <t>"{Name} dish" screen</t>
   </si>
   <si>
-    <t>1. "{Name}" dish screen
-2. Back button
-3. [Редактировать] button
-4. "{Name}" dish Picture
-5. "{Name}" dish
-6. Content info
-7. Tab bar
-8. {Name}Tab bar button</t>
-  </si>
-  <si>
     <t>"Edit {Name} dish" screen</t>
-  </si>
-  <si>
-    <t>1. "Редактировать блюдо" screen
-2. Back button 
-3. [Удалить] button
-4. [Сохранить] button
-5. "{Name}" dish field
-6. Content info
-7. Segment control
-8. Selected segment
-9. [Выбрать фото] button</t>
-  </si>
-  <si>
-    <t>1. "Мои блюда" screen
-2. Group name
-3. Dishes list
-4. {Name} dish
-5. Tab bar
-6. {Name}Tab bar button
-7. Add button</t>
   </si>
   <si>
     <t>"New dish" screen</t>
@@ -162,8 +132,41 @@
   </si>
   <si>
     <t>1. [Войти через Google] button
-2. [Зарегистрироваться] button
+2. [Войти чере AppleID] button
 3. [Продолжить без регистрации] button</t>
+  </si>
+  <si>
+    <t>1. "Мои блюда" screen
+2. Group name
+3. Dishes list
+4. {Name} dish item
+5. Tab bar
+6. {Name}Tab bar button
+7. Add button</t>
+  </si>
+  <si>
+    <t>1. "{Name}" dish screen
+2. Back button
+3. [Редактировать] button
+4. "{Name}" dish Picture
+5. "{Name}" dish
+6. Content info field
+7. Tab bar
+8. {Name}Tab bar button</t>
+  </si>
+  <si>
+    <t>1. "Редактировать блюдо" screen
+2. Back button 
+3. [Удалить] button
+4. [Сохранить] button
+5. "{Name}" dish field
+6. Content info field
+7. Segment control
+8. Selected segment
+9. [Выбрать фото] button</t>
+  </si>
+  <si>
+    <t>"Inviting in the {Name} group" screen</t>
   </si>
 </sst>
 </file>
@@ -285,6 +288,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -293,13 +303,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -911,22 +914,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2802960</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>4141470</xdr:rowOff>
+      <xdr:colOff>2796541</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>15929</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Рисунок 15">
+        <xdr:cNvPr id="15" name="Рисунок 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DF3A1BE-732D-461C-BD89-54EDF8D984F0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{085EB2B2-F71F-4EA0-B561-F00830E24ADC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -949,8 +952,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="504825"/>
-          <a:ext cx="2799150" cy="4143375"/>
+          <a:off x="1" y="504825"/>
+          <a:ext cx="2800350" cy="4170734"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1271,8 +1274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3B538B-1E03-4212-A4DA-A3DBB822E499}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1298,23 +1301,23 @@
       </c>
       <c r="B1" s="5"/>
     </row>
-    <row r="2" spans="1:13" s="10" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="9"/>
+    <row r="2" spans="1:13" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="8"/>
     </row>
-    <row r="3" spans="1:13" s="10" customFormat="1" ht="327.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" s="6" customFormat="1" ht="327.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3"/>
-      <c r="B3" s="11" t="s">
-        <v>23</v>
+      <c r="B3" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="9"/>
+      <c r="B4" s="8"/>
     </row>
     <row r="5" spans="1:13" ht="328.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
@@ -1323,99 +1326,102 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="9"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:13" ht="342" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="9"/>
+      <c r="A8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="8"/>
     </row>
     <row r="9" spans="1:13" ht="339" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="11"/>
+      <c r="E10" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="6" t="s">
+      <c r="H10" s="10"/>
+      <c r="I10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="7"/>
-      <c r="I10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L10" s="8"/>
-      <c r="M10" s="7"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" s="11"/>
+      <c r="M10" s="10"/>
     </row>
     <row r="11" spans="1:13" ht="365.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="H11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="2" t="s">
+      <c r="J11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M11" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="C10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
adding E2E test, need to upd Glossary
</commit_message>
<xml_diff>
--- a/DesignDocs/Glossary_Random4Dinner.xlsx
+++ b/DesignDocs/Glossary_Random4Dinner.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EnyFood\Random4Dinner\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5624E8B-E9BF-4F03-8CCA-CADC59E8BBB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EB3811-5497-4729-8645-DDEF3E90CC80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25740" yWindow="1080" windowWidth="24960" windowHeight="20085" xr2:uid="{8C7EFB95-537E-4066-989B-733ADEACC89B}"/>
+    <workbookView xWindow="-44100" yWindow="795" windowWidth="36525" windowHeight="12330" xr2:uid="{8C7EFB95-537E-4066-989B-733ADEACC89B}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист2" sheetId="2" r:id="rId1"/>
@@ -109,23 +109,7 @@
     <t>"New receipt" screen</t>
   </si>
   <si>
-    <t>1. [Отмена] button 
-2. [Добавить] button 
-3. "{Name} receipt field
-4. Adding category field
-5. Contetn info
-6. YouTube/Website link field
-7. Stepper
-8. Ingredients field
-9. Portion details</t>
-  </si>
-  <si>
     <t>"{Name} receipt" screen</t>
-  </si>
-  <si>
-    <t>1. Edit button
-2. Stepper
-3. Counter</t>
   </si>
   <si>
     <t>"Registration" screen</t>
@@ -167,6 +151,23 @@
   </si>
   <si>
     <t>"Inviting in the {Name} group" screen</t>
+  </si>
+  <si>
+    <t>1. Edit button
+2. Stepper
+3. Counter
+4. Back button</t>
+  </si>
+  <si>
+    <t>1. [Отмена] button 
+2. [Добавить] button 
+3. "{Name} receipt field
+4. Category Picker
+5. Contetn info field
+6. Link field
+7. Stepper
+8. Ingredients field
+9. Proportions stepper</t>
   </si>
 </sst>
 </file>
@@ -863,56 +864,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>3101340</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>4631055</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="30" name="Рисунок 29">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAC151BE-3D36-4CE8-9CE8-116AE353C4C1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="20354925" y="13992225"/>
-          <a:ext cx="3105150" cy="4629150"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>2</xdr:row>
@@ -938,7 +889,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -968,6 +919,50 @@
             </a14:hiddenFill>
           </a:ext>
         </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1971674</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>3133724</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>4529149</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Рисунок 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{474FCC3E-AB2F-4CD6-A038-FD3F3238C8CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20354924" y="18373725"/>
+          <a:ext cx="3133725" cy="4529149"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1274,8 +1269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3B538B-1E03-4212-A4DA-A3DBB822E499}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="F8" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1303,14 +1298,14 @@
     </row>
     <row r="2" spans="1:13" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" s="8"/>
     </row>
     <row r="3" spans="1:13" s="6" customFormat="1" ht="327.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3"/>
       <c r="B3" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -1341,13 +1336,13 @@
     </row>
     <row r="7" spans="1:13" ht="342" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -1371,7 +1366,7 @@
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="9" t="s">
@@ -1379,7 +1374,7 @@
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="9" t="s">
@@ -1402,10 +1397,10 @@
         <v>13</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>